<commit_message>
se hace festure/rental car
</commit_message>
<xml_diff>
--- a/Devco-automation/src/test/resources/data/DataFile.xlsx
+++ b/Devco-automation/src/test/resources/data/DataFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\Devco project\Devco-automation\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186803D7-989E-41F8-93A1-06C38B3F2AC2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6BFAD2-8EDE-43F5-A0AA-E954ACDE5489}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8CF633A6-09B7-4C64-BA02-675630DEA68C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8CF633A6-09B7-4C64-BA02-675630DEA68C}"/>
   </bookViews>
   <sheets>
     <sheet name="Devco_test" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>ID_Prueba</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>Hernanmalave%s@gmail.com</t>
+  </si>
+  <si>
+    <t>placeDelivery</t>
+  </si>
+  <si>
+    <t>Miami Beach, Florida, Estados Unidos</t>
   </si>
 </sst>
 </file>
@@ -436,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F6A1805-860E-453D-9C3B-A8B7A1659A20}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -448,10 +454,11 @@
     <col min="5" max="5" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="16.5546875" customWidth="1"/>
-    <col min="10" max="10" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.5546875" customWidth="1"/>
+    <col min="11" max="11" width="33.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -482,8 +489,11 @@
       <c r="J1" t="s">
         <v>1</v>
       </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -514,8 +524,11 @@
       <c r="J2" t="s">
         <v>2</v>
       </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F14" t="s">
         <v>16</v>
       </c>

</xml_diff>